<commit_message>
Signed-off-by: duan bin <binbin.duan@pisofttech.com> 修改格式
</commit_message>
<xml_diff>
--- a/各大平台SDK对比/SDK 对比.xlsx
+++ b/各大平台SDK对比/SDK 对比.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>微博</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,23 +30,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Access Token expiration time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>60 days</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1 hour</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expiration time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Access Token </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +65,26 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,18 +96,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -415,15 +438,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>